<commit_message>
update signup confirmation and member create
</commit_message>
<xml_diff>
--- a/public/MyPageSortedMemberList.xlsx
+++ b/public/MyPageSortedMemberList.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
-  <si>
-    <t>Sorted Expired Member List as of 02/11/2021</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+  <si>
+    <t>Sorted Member List as of 02/11/2021</t>
   </si>
   <si>
     <t>I.D</t>
@@ -38,6 +38,42 @@
     <t>Expiration Date</t>
   </si>
   <si>
+    <t>TOKO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">morimura </t>
+  </si>
+  <si>
+    <t>tokoko0415@gmail.com</t>
+  </si>
+  <si>
+    <t>02-23-2021  03:18:40 PM</t>
+  </si>
+  <si>
+    <t>KIZUKU IW</t>
+  </si>
+  <si>
+    <t>yamashita</t>
+  </si>
+  <si>
+    <t>ykizuku+1@gmail.com</t>
+  </si>
+  <si>
+    <t>02-19-2021  11:09:36 PM</t>
+  </si>
+  <si>
+    <t>SHIGEKI</t>
+  </si>
+  <si>
+    <t>kudo</t>
+  </si>
+  <si>
+    <t>sigeki1968@gmail.com</t>
+  </si>
+  <si>
+    <t>02-19-2021  08:55:18 PM</t>
+  </si>
+  <si>
     <t>KANTA</t>
   </si>
   <si>
@@ -48,54 +84,6 @@
   </si>
   <si>
     <t>02-09-2021  11:29:32 PM</t>
-  </si>
-  <si>
-    <t>Narumi</t>
-  </si>
-  <si>
-    <t>Nagakubo</t>
-  </si>
-  <si>
-    <t>narumi.763@hotmail.co.jp</t>
-  </si>
-  <si>
-    <t>01-23-2021  10:29:36 PM</t>
-  </si>
-  <si>
-    <t>SHIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akagawa </t>
-  </si>
-  <si>
-    <t>urunaru76767@yahoo.co.jp</t>
-  </si>
-  <si>
-    <t>01-19-2021  09:08:42 PM</t>
-  </si>
-  <si>
-    <t>YUKARI</t>
-  </si>
-  <si>
-    <t>Hikita</t>
-  </si>
-  <si>
-    <t>edelira49@outlook.jp</t>
-  </si>
-  <si>
-    <t>01-19-2021  03:51:38 PM</t>
-  </si>
-  <si>
-    <t>Mariko</t>
-  </si>
-  <si>
-    <t>Kanamaru</t>
-  </si>
-  <si>
-    <t>junko_62@icloud.com</t>
-  </si>
-  <si>
-    <t>12-14-2020  08:33:10 PM</t>
   </si>
 </sst>
 </file>
@@ -478,10 +466,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B7" sqref="B7:G7"/>
+      <selection activeCell="B6" sqref="B6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -518,7 +506,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="3">
-        <v>19509</v>
+        <v>19714</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -530,7 +518,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="3">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>10</v>
@@ -538,7 +526,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="B4" s="3">
-        <v>15244</v>
+        <v>19283</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
@@ -550,7 +538,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="3">
-        <v>30.0</v>
+        <v>3.0</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>14</v>
@@ -558,7 +546,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" s="3">
-        <v>8994</v>
+        <v>16400</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
@@ -570,7 +558,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="3">
-        <v>30.0</v>
+        <v>1.0</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>18</v>
@@ -578,7 +566,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="B6" s="3">
-        <v>19364</v>
+        <v>19509</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>19</v>
@@ -590,30 +578,10 @@
         <v>21</v>
       </c>
       <c r="F6" s="3">
-        <v>30.0</v>
+        <v>1.0</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="3">
-        <v>18159</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="3">
-        <v>50.0</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>